<commit_message>
google Q222 and other updates
</commit_message>
<xml_diff>
--- a/700 HK.xlsx
+++ b/700 HK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD20D1C-7010-478E-8850-303DBFA64C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B13923-84FD-487A-8D12-837BA59FFEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14370" yWindow="0" windowWidth="14505" windowHeight="15210" activeTab="1" xr2:uid="{C183CDF4-DAE3-4211-A459-AE4D0C2142B8}"/>
+    <workbookView xWindow="9570" yWindow="1875" windowWidth="18810" windowHeight="13215" xr2:uid="{C183CDF4-DAE3-4211-A459-AE4D0C2142B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -791,7 +791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E1D774-2E12-4746-88E6-1A6120E6AF7B}">
   <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -974,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666C0D08-E52C-4128-A040-0E26B040CE26}">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>